<commit_message>
#9 treat x columns as notes
</commit_message>
<xml_diff>
--- a/tests/testthat/test_data/impfmonitoring_three_notes.xlsx
+++ b/tests/testthat/test_data/impfmonitoring_three_notes.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{ADD9B314-2DCD-4145-8B76-5A09B82CD2E2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AD65D5E-E7E1-F84E-88C7-B9AB295C40AC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="460" windowWidth="28520" windowHeight="12600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="39">
   <si>
     <t>Bayern</t>
   </si>
@@ -143,6 +143,18 @@
   </si>
   <si>
     <t>Sachsen***</t>
+  </si>
+  <si>
+    <t>blabla</t>
+  </si>
+  <si>
+    <t>another note</t>
+  </si>
+  <si>
+    <t>bar</t>
+  </si>
+  <si>
+    <t>test</t>
   </si>
 </sst>
 </file>
@@ -747,7 +759,7 @@
       </c>
       <c r="B6" s="18">
         <f ca="1">TODAY()</f>
-        <v>44196</v>
+        <v>44200</v>
       </c>
       <c r="C6" s="19" t="s">
         <v>28</v>
@@ -791,10 +803,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8185A2DF-1594-45F9-85B9-EB1F8407882D}">
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -804,7 +816,7 @@
     <col min="7" max="7" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>12</v>
       </c>
@@ -827,7 +839,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -849,8 +861,14 @@
       <c r="G2" s="8">
         <v>933</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
@@ -872,8 +890,11 @@
       <c r="G3" s="17">
         <v>5314</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -896,7 +917,7 @@
         <v>4899</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>2</v>
       </c>
@@ -919,7 +940,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>31</v>
       </c>
@@ -942,7 +963,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
@@ -965,7 +986,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>32</v>
       </c>
@@ -988,7 +1009,7 @@
         <v>3825</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>5</v>
       </c>
@@ -1011,7 +1032,7 @@
         <v>3231</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>6</v>
       </c>
@@ -1034,7 +1055,7 @@
         <v>794</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>7</v>
       </c>
@@ -1057,7 +1078,7 @@
         <v>8622</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>9</v>
       </c>
@@ -1080,7 +1101,7 @@
         <v>1273</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>10</v>
       </c>
@@ -1103,7 +1124,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>34</v>
       </c>
@@ -1125,8 +1146,11 @@
       <c r="G14" s="8">
         <v>192</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>33</v>
       </c>
@@ -1149,7 +1173,7 @@
         <v>3942</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
Deal with unnamed notes columns  (#11)
* #9 treat x columns as notes

* news md

* correct news md

* import tidyr

* add tidyr
</commit_message>
<xml_diff>
--- a/tests/testthat/test_data/impfmonitoring_three_notes.xlsx
+++ b/tests/testthat/test_data/impfmonitoring_three_notes.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{ADD9B314-2DCD-4145-8B76-5A09B82CD2E2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AD65D5E-E7E1-F84E-88C7-B9AB295C40AC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="460" windowWidth="28520" windowHeight="12600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="39">
   <si>
     <t>Bayern</t>
   </si>
@@ -143,6 +143,18 @@
   </si>
   <si>
     <t>Sachsen***</t>
+  </si>
+  <si>
+    <t>blabla</t>
+  </si>
+  <si>
+    <t>another note</t>
+  </si>
+  <si>
+    <t>bar</t>
+  </si>
+  <si>
+    <t>test</t>
   </si>
 </sst>
 </file>
@@ -747,7 +759,7 @@
       </c>
       <c r="B6" s="18">
         <f ca="1">TODAY()</f>
-        <v>44196</v>
+        <v>44200</v>
       </c>
       <c r="C6" s="19" t="s">
         <v>28</v>
@@ -791,10 +803,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8185A2DF-1594-45F9-85B9-EB1F8407882D}">
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -804,7 +816,7 @@
     <col min="7" max="7" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>12</v>
       </c>
@@ -827,7 +839,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -849,8 +861,14 @@
       <c r="G2" s="8">
         <v>933</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
@@ -872,8 +890,11 @@
       <c r="G3" s="17">
         <v>5314</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -896,7 +917,7 @@
         <v>4899</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>2</v>
       </c>
@@ -919,7 +940,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>31</v>
       </c>
@@ -942,7 +963,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
@@ -965,7 +986,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>32</v>
       </c>
@@ -988,7 +1009,7 @@
         <v>3825</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>5</v>
       </c>
@@ -1011,7 +1032,7 @@
         <v>3231</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>6</v>
       </c>
@@ -1034,7 +1055,7 @@
         <v>794</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>7</v>
       </c>
@@ -1057,7 +1078,7 @@
         <v>8622</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>9</v>
       </c>
@@ -1080,7 +1101,7 @@
         <v>1273</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>10</v>
       </c>
@@ -1103,7 +1124,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>34</v>
       </c>
@@ -1125,8 +1146,11 @@
       <c r="G14" s="8">
         <v>192</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>33</v>
       </c>
@@ -1149,7 +1173,7 @@
         <v>3942</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>8</v>
       </c>

</xml_diff>